<commit_message>
modif url VS 9149f258720dc0c2adfe44ec4166c221ec120d28
</commit_message>
<xml_diff>
--- a/ig/sd-error-url-vs-research-study-status/eclaire-study-status-concept-map.xlsx
+++ b/ig/sd-error-url-vs-research-study-status/eclaire-study-status-concept-map.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-09-01T14:00:04+00:00</t>
+    <t>2023-09-01T14:24:41+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -96,7 +96,7 @@
     <t>Target</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/R4/valueset-research-study-status</t>
+    <t>http://hl7.org/fhir/ValueSet/research-study-status</t>
   </si>
   <si>
     <t>Display</t>

</xml_diff>